<commit_message>
fix check for current holdings
</commit_message>
<xml_diff>
--- a/data/2023/fid/FID-ALT-AY-DE-16.xlsx
+++ b/data/2023/fid/FID-ALT-AY-DE-16.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="222">
   <si>
     <t>ZDBDID</t>
   </si>
@@ -157,145 +157,148 @@
     <t>1.1962 - 29.1990,1/2 ; Series nova, 1 (2019)-</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>DE-1a;DE-12</t>
+  </si>
+  <si>
+    <t>2402717-0</t>
+  </si>
+  <si>
+    <t>Pražské egyptologické studie</t>
+  </si>
+  <si>
+    <t>Univ. Karlova</t>
+  </si>
+  <si>
+    <t>Praha</t>
+  </si>
+  <si>
+    <t>cze</t>
+  </si>
+  <si>
+    <t>1214-3189</t>
+  </si>
+  <si>
+    <t>FID-ALT-AY-DE-16</t>
+  </si>
+  <si>
+    <t>Suplementa</t>
+  </si>
+  <si>
+    <t>2003 - 2004</t>
+  </si>
+  <si>
+    <t>2558986-6</t>
+  </si>
+  <si>
+    <t>Saqqara newsletter</t>
+  </si>
+  <si>
+    <t>[Verlag nicht ermittelbar]</t>
+  </si>
+  <si>
+    <t>Leiden</t>
+  </si>
+  <si>
+    <t>930</t>
+  </si>
+  <si>
+    <t>1.2003 -</t>
+  </si>
+  <si>
+    <t>2841985-6</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>The Brill Dictionary of Ancient Greek</t>
+  </si>
+  <si>
+    <t>Brill</t>
+  </si>
+  <si>
+    <t>930;870;880</t>
+  </si>
+  <si>
+    <t>FID-ALT-DE-12;FID-ALT-KA-DE-16;FID-ALT-AY-DE-16</t>
+  </si>
+  <si>
+    <t>Nachgewiesen 2015 -</t>
+  </si>
+  <si>
+    <t>http://dictionaries.brillonline.com/montanari;http://dbis.uni-regensburg.de/frontdoor.php?titel_id=100901</t>
+  </si>
+  <si>
+    <t>2870450-2</t>
+  </si>
+  <si>
+    <t>The journal of Ancient Egyptian architecture</t>
+  </si>
+  <si>
+    <t>[Erscheinungsort nicht ermittelbar]</t>
+  </si>
+  <si>
+    <t>2472-999X</t>
+  </si>
+  <si>
+    <t>Volume 1 (July/December 2016)-</t>
+  </si>
+  <si>
+    <t>http://www.egyptian-architecture.com/;http://www.bibliothek.uni-regensburg.de/ezeit/?2870450</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>DE-12;DE-19;DE-20;DE-862;DE-863;DE-26;DE-29;DE-1102;DE-946;DE-90;DE-355;DE-898;DE-155;DE-384;DE-Aug4;DE-37;DE-473;DE-703;DE-739;DE-824;DE-573;DE-150;DE-634;DE-706;DE-523;DE-Re13</t>
+  </si>
+  <si>
+    <t>2875945-X</t>
+  </si>
+  <si>
+    <t>Nile</t>
+  </si>
+  <si>
+    <t>NILE Magazine</t>
+  </si>
+  <si>
+    <t>[Great Britain]</t>
+  </si>
+  <si>
+    <t>2206-0502</t>
+  </si>
+  <si>
+    <t>#1 (April/May 2016)-</t>
+  </si>
+  <si>
+    <t>3100356-4</t>
+  </si>
+  <si>
+    <t>rb;b</t>
+  </si>
+  <si>
+    <t>CIPEG journal</t>
+  </si>
+  <si>
+    <t>Propylaeum, Heidelberg University Library</t>
+  </si>
+  <si>
+    <t>Heidelberg</t>
+  </si>
+  <si>
+    <t>930;060</t>
+  </si>
+  <si>
+    <t>No. 5 (2021) [?]-</t>
+  </si>
+  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>DE-12</t>
-  </si>
-  <si>
-    <t>2402717-0</t>
-  </si>
-  <si>
-    <t>Pražské egyptologické studie</t>
-  </si>
-  <si>
-    <t>Univ. Karlova</t>
-  </si>
-  <si>
-    <t>Praha</t>
-  </si>
-  <si>
-    <t>cze</t>
-  </si>
-  <si>
-    <t>1214-3189</t>
-  </si>
-  <si>
-    <t>FID-ALT-AY-DE-16</t>
-  </si>
-  <si>
-    <t>Suplementa</t>
-  </si>
-  <si>
-    <t>2003 - 2004</t>
-  </si>
-  <si>
-    <t>2558986-6</t>
-  </si>
-  <si>
-    <t>Saqqara newsletter</t>
-  </si>
-  <si>
-    <t>[Verlag nicht ermittelbar]</t>
-  </si>
-  <si>
-    <t>Leiden</t>
-  </si>
-  <si>
-    <t>930</t>
-  </si>
-  <si>
-    <t>1.2003 -</t>
-  </si>
-  <si>
-    <t>2841985-6</t>
-  </si>
-  <si>
-    <t>online</t>
-  </si>
-  <si>
-    <t>The Brill Dictionary of Ancient Greek</t>
-  </si>
-  <si>
-    <t>Brill</t>
-  </si>
-  <si>
-    <t>930;870;880</t>
-  </si>
-  <si>
-    <t>FID-ALT-DE-12;FID-ALT-KA-DE-16;FID-ALT-AY-DE-16</t>
-  </si>
-  <si>
-    <t>Nachgewiesen 2015 -</t>
-  </si>
-  <si>
-    <t>http://dictionaries.brillonline.com/montanari;http://dbis.uni-regensburg.de/frontdoor.php?titel_id=100901</t>
-  </si>
-  <si>
-    <t>2870450-2</t>
-  </si>
-  <si>
-    <t>The journal of Ancient Egyptian architecture</t>
-  </si>
-  <si>
-    <t>[Erscheinungsort nicht ermittelbar]</t>
-  </si>
-  <si>
-    <t>2472-999X</t>
-  </si>
-  <si>
-    <t>Volume 1 (July/December 2016)-</t>
-  </si>
-  <si>
-    <t>http://www.egyptian-architecture.com/;http://www.bibliothek.uni-regensburg.de/ezeit/?2870450</t>
-  </si>
-  <si>
-    <t>LF</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>DE-12;DE-19;DE-20;DE-862;DE-863;DE-26;DE-29;DE-1102;DE-946;DE-90;DE-355;DE-898;DE-155;DE-384;DE-Aug4;DE-37;DE-473;DE-703;DE-739;DE-824;DE-573;DE-150;DE-634;DE-706;DE-523;DE-Re13</t>
-  </si>
-  <si>
-    <t>2875945-X</t>
-  </si>
-  <si>
-    <t>Nile</t>
-  </si>
-  <si>
-    <t>NILE Magazine</t>
-  </si>
-  <si>
-    <t>[Great Britain]</t>
-  </si>
-  <si>
-    <t>2206-0502</t>
-  </si>
-  <si>
-    <t>#1 (April/May 2016)-</t>
-  </si>
-  <si>
-    <t>3100356-4</t>
-  </si>
-  <si>
-    <t>rb;b</t>
-  </si>
-  <si>
-    <t>CIPEG journal</t>
-  </si>
-  <si>
-    <t>Propylaeum, Heidelberg University Library</t>
-  </si>
-  <si>
-    <t>Heidelberg</t>
-  </si>
-  <si>
-    <t>930;060</t>
-  </si>
-  <si>
-    <t>No. 5 (2021) [?]-</t>
   </si>
   <si>
     <t>DE-31</t>
@@ -1701,33 +1704,33 @@
         <v>32</v>
       </c>
       <c r="X9" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="Y9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -1742,7 +1745,7 @@
         <v>55</v>
       </c>
       <c r="L10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M10" t="s">
         <v>32</v>
@@ -1760,7 +1763,7 @@
         <v>32</v>
       </c>
       <c r="R10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S10" t="s">
         <v>32</v>
@@ -1786,7 +1789,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
         <v>65</v>
@@ -1795,13 +1798,13 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
         <v>31</v>
@@ -1837,10 +1840,10 @@
         <v>32</v>
       </c>
       <c r="R11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="S11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="T11" t="s">
         <v>78</v>
@@ -1858,36 +1861,36 @@
         <v>79</v>
       </c>
       <c r="Y11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F12" t="s">
         <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s">
         <v>32</v>
       </c>
       <c r="I12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J12" t="s">
         <v>62</v>
@@ -1914,10 +1917,10 @@
         <v>32</v>
       </c>
       <c r="R12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="S12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="T12" t="s">
         <v>78</v>
@@ -1940,25 +1943,25 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H13" t="s">
         <v>32</v>
@@ -1991,10 +1994,10 @@
         <v>32</v>
       </c>
       <c r="R13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="S13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T13" t="s">
         <v>32</v>
@@ -2017,7 +2020,7 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -2026,10 +2029,10 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F14" t="s">
         <v>61</v>
@@ -2041,7 +2044,7 @@
         <v>32</v>
       </c>
       <c r="I14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J14" t="s">
         <v>33</v>
@@ -2065,10 +2068,10 @@
         <v>32</v>
       </c>
       <c r="Q14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S14" t="s">
         <v>32</v>
@@ -2086,15 +2089,15 @@
         <v>32</v>
       </c>
       <c r="X14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Y14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
@@ -2106,7 +2109,7 @@
         <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F15" t="s">
         <v>91</v>
@@ -2118,7 +2121,7 @@
         <v>32</v>
       </c>
       <c r="I15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J15" t="s">
         <v>62</v>
@@ -2145,10 +2148,10 @@
         <v>32</v>
       </c>
       <c r="R15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="S15" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="T15" t="s">
         <v>78</v>
@@ -2171,7 +2174,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s">
         <v>65</v>
@@ -2180,16 +2183,16 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H16" t="s">
         <v>32</v>
@@ -2222,10 +2225,10 @@
         <v>32</v>
       </c>
       <c r="R16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="S16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="T16" t="s">
         <v>78</v>
@@ -2248,7 +2251,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
@@ -2257,16 +2260,16 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F17" t="s">
         <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H17" t="s">
         <v>32</v>
@@ -2275,7 +2278,7 @@
         <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K17" t="s">
         <v>55</v>
@@ -2299,10 +2302,10 @@
         <v>32</v>
       </c>
       <c r="R17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="S17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="T17" t="s">
         <v>78</v>
@@ -2317,30 +2320,30 @@
         <v>32</v>
       </c>
       <c r="X17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Y17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s">
         <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G18" t="s">
         <v>31</v>
@@ -2355,10 +2358,10 @@
         <v>32</v>
       </c>
       <c r="K18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M18" t="s">
         <v>32</v>
@@ -2379,7 +2382,7 @@
         <v>32</v>
       </c>
       <c r="S18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="T18" t="s">
         <v>32</v>
@@ -2402,7 +2405,7 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B19" t="s">
         <v>65</v>
@@ -2411,13 +2414,13 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E19" t="s">
         <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G19" t="s">
         <v>31</v>
@@ -2432,10 +2435,10 @@
         <v>62</v>
       </c>
       <c r="K19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M19" t="s">
         <v>32</v>
@@ -2456,7 +2459,7 @@
         <v>32</v>
       </c>
       <c r="S19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="T19" t="s">
         <v>32</v>
@@ -2479,7 +2482,7 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
         <v>65</v>
@@ -2488,16 +2491,16 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H20" t="s">
         <v>32</v>
@@ -2509,7 +2512,7 @@
         <v>62</v>
       </c>
       <c r="K20" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L20" t="s">
         <v>32</v>
@@ -2533,7 +2536,7 @@
         <v>32</v>
       </c>
       <c r="S20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T20" t="s">
         <v>32</v>
@@ -2556,22 +2559,22 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
         <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F21" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G21" t="s">
         <v>32</v>
@@ -2583,10 +2586,10 @@
         <v>32</v>
       </c>
       <c r="J21" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L21" t="s">
         <v>32</v>
@@ -2607,13 +2610,13 @@
         <v>32</v>
       </c>
       <c r="R21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="S21" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="U21" t="s">
         <v>32</v>
@@ -2633,16 +2636,16 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B22" t="s">
         <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E22" t="s">
         <v>67</v>
@@ -2651,19 +2654,19 @@
         <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
       </c>
       <c r="I22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L22" t="s">
         <v>32</v>
@@ -2678,7 +2681,7 @@
         <v>32</v>
       </c>
       <c r="P22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Q22" t="s">
         <v>32</v>
@@ -2687,10 +2690,10 @@
         <v>32</v>
       </c>
       <c r="S22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="T22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="U22" t="s">
         <v>32</v>
@@ -2710,7 +2713,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -2719,16 +2722,16 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E23" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F23" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G23" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -2761,7 +2764,7 @@
         <v>32</v>
       </c>
       <c r="R23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S23" t="s">
         <v>32</v>
@@ -2787,7 +2790,7 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
@@ -2796,13 +2799,13 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G24" t="s">
         <v>31</v>
@@ -2841,7 +2844,7 @@
         <v>32</v>
       </c>
       <c r="S24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="T24" t="s">
         <v>32</v>
@@ -2864,7 +2867,7 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
@@ -2873,13 +2876,13 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E25" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F25" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G25" t="s">
         <v>31</v>
@@ -2894,10 +2897,10 @@
         <v>62</v>
       </c>
       <c r="K25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M25" t="s">
         <v>32</v>
@@ -2918,7 +2921,7 @@
         <v>32</v>
       </c>
       <c r="S25" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="T25" t="s">
         <v>32</v>
@@ -2941,7 +2944,7 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -2950,13 +2953,13 @@
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E26" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F26" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G26" t="s">
         <v>31</v>
@@ -2974,7 +2977,7 @@
         <v>69</v>
       </c>
       <c r="L26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="M26" t="s">
         <v>32</v>
@@ -2995,7 +2998,7 @@
         <v>32</v>
       </c>
       <c r="S26" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="T26" t="s">
         <v>32</v>
@@ -3018,7 +3021,7 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -3027,13 +3030,13 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E27" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G27" t="s">
         <v>31</v>
@@ -3069,10 +3072,10 @@
         <v>32</v>
       </c>
       <c r="R27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="S27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="T27" t="s">
         <v>78</v>
@@ -3090,7 +3093,7 @@
         <v>79</v>
       </c>
       <c r="Y27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>